<commit_message>
Atualiza dados do modelo - roda modelo com dados de treino e teste
</commit_message>
<xml_diff>
--- a/tabelas/tipo_colunas.xlsx
+++ b/tabelas/tipo_colunas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t>coluna</t>
   </si>
@@ -46,9 +46,6 @@
     <t>TP_ST_CONCLUSAO</t>
   </si>
   <si>
-    <t>TP_ENSINO</t>
-  </si>
-  <si>
     <t>Q001</t>
   </si>
   <si>
@@ -77,21 +74,6 @@
   </si>
   <si>
     <t>NU_NOTA_MT</t>
-  </si>
-  <si>
-    <t>NU_NOTA_COMP1</t>
-  </si>
-  <si>
-    <t>NU_NOTA_COMP2</t>
-  </si>
-  <si>
-    <t>NU_NOTA_COMP3</t>
-  </si>
-  <si>
-    <t>NU_NOTA_COMP4</t>
-  </si>
-  <si>
-    <t>NU_NOTA_COMP5</t>
   </si>
   <si>
     <t>NU_NOTA_REDACAO</t>
@@ -473,7 +455,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -495,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -506,7 +488,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -517,7 +499,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -528,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -539,7 +521,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -550,7 +532,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -561,7 +543,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -572,7 +554,7 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -583,7 +565,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -594,7 +576,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -605,7 +587,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -616,7 +598,7 @@
         <v>13</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -627,7 +609,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -638,7 +620,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -649,7 +631,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -660,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -671,7 +653,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -682,7 +664,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -693,7 +675,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -704,73 +686,7 @@
         <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="1">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" s="1">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="1">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
         <v>26</v>
-      </c>
-      <c r="C26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" s="1">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualiza modelo e graficos para projeto escrito
</commit_message>
<xml_diff>
--- a/tabelas/tipo_colunas.xlsx
+++ b/tabelas/tipo_colunas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>coluna</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>TP_NACIONALIDADE</t>
-  </si>
-  <si>
-    <t>NO_MUNICIPIO_RESIDENCIA</t>
   </si>
   <si>
     <t>SG_UF_RESIDENCIA</t>
@@ -455,7 +452,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -477,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -488,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -499,7 +496,7 @@
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -510,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -521,7 +518,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -532,7 +529,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -543,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -565,7 +562,7 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -576,7 +573,7 @@
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -587,7 +584,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -631,7 +628,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -642,7 +639,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -653,7 +650,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -664,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -675,18 +672,7 @@
         <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>